<commit_message>
updated MDP diagram, fraud feature labels
</commit_message>
<xml_diff>
--- a/Guide/Diagram 3 - Fraud Risk Score Worksheet.xlsx
+++ b/Guide/Diagram 3 - Fraud Risk Score Worksheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l\individual-ivwangYW\5100CS_Group_Final_Project_Expense-AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l\individual-ivwangYW\5100CS_Group_Final_Project_Expense-AI\Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA4E4DF-A61D-4B00-B2D4-622AA685516F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5E0FB6-EDDF-495B-A720-13ABF083F377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EA238343-1867-4C18-9077-45F90A0BC4CD}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>score = 0 if all of the following is 0</t>
   </si>
   <si>
-    <t xml:space="preserve">Fraud Risk Score to be classified to :    5/10/0   </t>
-  </si>
-  <si>
     <t xml:space="preserve">score = 5 if </t>
   </si>
   <si>
@@ -67,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve">layers </t>
-  </si>
-  <si>
-    <t>Class (0,5,10)</t>
   </si>
   <si>
     <t>loss function</t>
@@ -305,6 +299,66 @@
 Sudden Changes in Behavior: Abrupt changes in reimbursement behavior, such as a sudden increase in claims or a change in the types of expenses being claimed.</t>
   </si>
   <si>
+    <t xml:space="preserve">a value  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">input: db中的每个同样的人同样的expense category的future invoice amount   | funtion:   parameters:  history      </t>
+  </si>
+  <si>
+    <t>Invoice Date falls outside of Project Duration Dates</t>
+  </si>
+  <si>
+    <t>Design a program(input: Project Duration_startDate, ProjectDuration_endDate,current  Invoice Date|output: 0/1</t>
+  </si>
+  <si>
+    <t>dubious merchants</t>
+  </si>
+  <si>
+    <t>how do we determin if a score should be evaluated to 0,5, or 10?       Consider each potential fraud activity's</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Impact on Decision-Making: Consider how the fraud risk score will be used in decision-making. If a higher score leads to more stringent actions (e.g., additional scrutiny, investigation, or denial of reimbursement), reserve the highest scores for situations where the risk is deemed most critical.</t>
+  </si>
+  <si>
+    <t>Costs and Consequences:  If assigning a higher score results in more significant consequences, such as the denial of a valid reimbursement, you may want to set the threshold cautiously.</t>
+  </si>
+  <si>
+    <t>sources - fraud detection:</t>
+  </si>
+  <si>
+    <t>fraud detection</t>
+  </si>
+  <si>
+    <t>https://trenton3983.github.io/files/projects/2019-07-19_fraud_detection_python/2019-07-19_fraud_detection_python.html</t>
+  </si>
+  <si>
+    <t>create nn with custom weight in tensorflow or pytorch</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/57803287/how-to-create-custom-neural-network-with-custom-weight-initialization-in-tensorf</t>
+  </si>
+  <si>
+    <t>activation functions in neural network</t>
+  </si>
+  <si>
+    <t>https://www.v7labs.com/blog/neural-networks-activation-functions</t>
+  </si>
+  <si>
+    <t>Creating a custom Neural Network with PyTorch</t>
+  </si>
+  <si>
+    <t>https://medium.com/academy-eldoradocps/creating-a-custom-neural-network-with-pytorch-fd3621705d32</t>
+  </si>
+  <si>
+    <t>Using AI to Prevent Supplier Invoice Fraud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraud Risk Score to be classified to :    0/3/6/10 </t>
+  </si>
+  <si>
+    <t>Class (0,3,6,10)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -337,17 +391,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and a program (input: prediction of future invoice amount at future dates based on historical data including all invoice amounts and invoice dates for same Expense Category claimed by same employeeID over the last 3 years   from the database, and the current invoice date and amount|  Output:  Standard Deviation -see standard deviation calculation Word file in 5100 local folder for final project)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
+      <t xml:space="preserve"> and a program (input: prediction of future invoice amount at future dates based on historical data including all invoice amounts and invoice dates for same Expense Category claimed by same employeeID over the last 3 years   from the database, and the current invoice date and amount|  Output:   variance between current invoice Amount and the predicted amount for same expence category for same employee</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -358,62 +412,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note:  within  1 year the claims can only cover a few months, need to revise formula</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">a value  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">input: db中的每个同样的人同样的expense category的future invoice amount   | funtion:   parameters:  history      </t>
-  </si>
-  <si>
-    <t>Invoice Date falls outside of Project Duration Dates</t>
-  </si>
-  <si>
-    <t>Design a program(input: Project Duration_startDate, ProjectDuration_endDate,current  Invoice Date|output: 0/1</t>
-  </si>
-  <si>
-    <t>dubious merchants</t>
-  </si>
-  <si>
-    <t>how do we determin if a score should be evaluated to 0,5, or 10?       Consider each potential fraud activity's</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Impact on Decision-Making: Consider how the fraud risk score will be used in decision-making. If a higher score leads to more stringent actions (e.g., additional scrutiny, investigation, or denial of reimbursement), reserve the highest scores for situations where the risk is deemed most critical.</t>
-  </si>
-  <si>
-    <t>Costs and Consequences:  If assigning a higher score results in more significant consequences, such as the denial of a valid reimbursement, you may want to set the threshold cautiously.</t>
-  </si>
-  <si>
-    <t>sources - fraud detection:</t>
-  </si>
-  <si>
-    <t>fraud detection</t>
-  </si>
-  <si>
-    <t>https://trenton3983.github.io/files/projects/2019-07-19_fraud_detection_python/2019-07-19_fraud_detection_python.html</t>
-  </si>
-  <si>
-    <t>create nn with custom weight in tensorflow or pytorch</t>
-  </si>
-  <si>
-    <t>https://stackoverflow.com/questions/57803287/how-to-create-custom-neural-network-with-custom-weight-initialization-in-tensorf</t>
-  </si>
-  <si>
-    <t>activation functions in neural network</t>
-  </si>
-  <si>
-    <t>https://www.v7labs.com/blog/neural-networks-activation-functions</t>
-  </si>
-  <si>
-    <t>Creating a custom Neural Network with PyTorch</t>
-  </si>
-  <si>
-    <t>https://medium.com/academy-eldoradocps/creating-a-custom-neural-network-with-pytorch-fd3621705d32</t>
-  </si>
-  <si>
-    <t>Using AI to Prevent Supplier Invoice Fraud</t>
+      <t>Note:  In database, data might not cover full past 3 years,  need to make sure that the prediction function don't run into bugs if data covers less length of time</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -860,8 +860,8 @@
   </sheetPr>
   <dimension ref="C4:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="E22" zoomScale="136" zoomScaleNormal="100" zoomScaleSheetLayoutView="136" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="E28" zoomScale="136" zoomScaleNormal="100" zoomScaleSheetLayoutView="136" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,64 +892,64 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
         <v>5</v>
-      </c>
-      <c r="K17" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="18" spans="4:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>8</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" t="s">
         <v>10</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>11</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" t="s">
         <v>12</v>
-      </c>
-      <c r="J18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="4:11" ht="30" x14ac:dyDescent="0.25">
       <c r="E20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -957,13 +957,13 @@
     </row>
     <row r="21" spans="4:11" ht="180" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -971,13 +971,13 @@
     </row>
     <row r="22" spans="4:11" ht="75" x14ac:dyDescent="0.25">
       <c r="E22" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H22">
         <v>10</v>
@@ -985,156 +985,156 @@
     </row>
     <row r="23" spans="4:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="G23" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" t="s">
         <v>26</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="24" spans="4:11" ht="60" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="G24" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="4:11" ht="195" x14ac:dyDescent="0.25">
       <c r="E26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="27" spans="4:11" ht="105" x14ac:dyDescent="0.25">
       <c r="E27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" ht="270" x14ac:dyDescent="0.25">
+      <c r="E28" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F28" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="4:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="E28" s="8" t="s">
+      <c r="H28" t="s">
         <v>39</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H28" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="29" spans="4:11" ht="60" x14ac:dyDescent="0.25">
       <c r="E29" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
       <c r="E30" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E40" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E42" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>